<commit_message>
sửa lại nội dung đã được review
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat nguoi dung/AS0053_Cap nhat nhan vien.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat nguoi dung/AS0053_Cap nhat nhan vien.xlsx
@@ -21,11 +21,11 @@
     <sheet name="Help" sheetId="6" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Data Input'!$A$1:$N$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Data Input'!$A$1:$N$53</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="5">'Func Spec'!$A$1:$J$45</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">Help!$A$1:$K$62</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'Input Check'!$A$1:$P$54</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">'Item Screen'!$A$1:$R$59</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Item Screen'!$A$1:$R$56</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Layout Screen'!$A$1:$J$87</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Update History'!$A$1:$J$43</definedName>
   </definedNames>
@@ -1087,7 +1087,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="240">
   <si>
     <t>Detail Design</t>
   </si>
@@ -1766,12 +1766,6 @@
     <t>Mật khẩu</t>
   </si>
   <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Nhập lại mật khẩu</t>
-  </si>
-  <si>
     <t>SID</t>
   </si>
   <si>
@@ -1790,12 +1784,6 @@
     <t>Ver 2.0</t>
   </si>
   <si>
-    <t>Dùng chung</t>
-  </si>
-  <si>
-    <t>IsCommon</t>
-  </si>
-  <si>
     <t>CustomizeIndex</t>
   </si>
   <si>
@@ -1824,9 +1812,6 @@
   </si>
   <si>
     <t>I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-Enabled khi có nhiều hơn một Division </t>
   </si>
   <si>
     <t>Sử dụng màn hình này để:
@@ -1859,50 +1844,19 @@
 -&gt;Cập nhật thông tin người dùng</t>
   </si>
   <si>
-    <t>IF EXISTS (SELECT TOP 1 1 FROM sysobjects WHERE [name] = 'AT1103' AND xtype = 'U')
-    BEGIN
-        IF NOT EXISTS (SELECT TOP 1 1 FROM syscolumns col INNER JOIN sysobjects tab
-        ON col.id = tab.id WHERE tab.name = 'AT1103' AND col.name = 'SipID')
-        ALTER TABLE AT1103 ADD SipID NVARCHAR(50) NULL
-    END</t>
-  </si>
-  <si>
-    <t>IF EXISTS (SELECT TOP 1 1 FROM sysobjects WHERE [name] = 'AT1103' AND xtype = 'U')
-    BEGIN
-        IF NOT EXISTS (SELECT TOP 1 1 FROM syscolumns col INNER JOIN sysobjects tab
-        ON col.id = tab.id WHERE tab.name = 'AT1103' AND col.name = 'SipPassword')
-        ALTER TABLE AT1103 ADD SipPassword NVARCHAR(50) NULL
-    END</t>
-  </si>
-  <si>
     <t>@SQL0001</t>
   </si>
   <si>
-    <t>@SQL0002</t>
-  </si>
-  <si>
     <t>* Trường hợp Add</t>
   </si>
   <si>
     <t>Trường hợp Edit và View</t>
   </si>
   <si>
-    <t>Disabled khi ở màn hình Edit và View</t>
-  </si>
-  <si>
-    <t>Thêm mới trường SipPassword vào AT1103 áp dụng cho CustomizeIndex 51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thêm mới trường SipID vào AT1103 áp dụng cho CustomizeIndex 51 </t>
-  </si>
-  <si>
     <t>Textbox này được thêm mới trong màn hình cũ. Disabled khi ở màn hình Edit</t>
   </si>
   <si>
     <t xml:space="preserve">EmployeeID, FullName, DepartmentID, EmployeeTypeID, HireDate, EndDate, BirthDay, Address, Tel, Fax, Email, IsUserID, SipID, SipPassword </t>
-  </si>
-  <si>
-    <t>@SQL0003</t>
   </si>
   <si>
     <t>INSERT INTO AT1103(DivisionID, EmployeeID, FullName,
@@ -1932,13 +1886,13 @@
 @@SipID @@SipPassword</t>
   </si>
   <si>
-    <t>Sửa lại câu SQL Insert into. Chỉ dùng cho CustomizeIndex = 51. Thực thi @SQL003 khi thêm mới một người dùng trong Form AS0053</t>
-  </si>
-  <si>
     <t>CustomizeIndex = 51 (Hoàng Trần)
 - Sheet Layout: thêm 2 trường SIP và Mật khẩu
 - Sheet Item Sreen: thêm 5 trường Mật khẩu, Nhập lại mật khẩu, SIP, Mật khẩu và Dùng chung
-- Sheet Data Input: Thêm câu @SQL0001, @SQL0002, @SQL0003</t>
+- Sheet Data Input: Thêm câu @SQL0001</t>
+  </si>
+  <si>
+    <t>Sửa lại câu SQL Insert into.Thực thi @SQL0001 khi thêm mới một người dùng trong Form AS0053</t>
   </si>
 </sst>
 </file>
@@ -2311,7 +2265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="166">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2658,6 +2612,39 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2667,39 +2654,6 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2735,15 +2689,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3184,7 +3129,7 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:J7"/>
+      <selection activeCell="E6" sqref="E6:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3242,7 +3187,7 @@
         <v>145</v>
       </c>
       <c r="F2" s="34" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="G2" s="30" t="s">
         <v>4</v>
@@ -3315,7 +3260,7 @@
         <v>210</v>
       </c>
       <c r="E6" s="111" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="F6" s="112"/>
       <c r="G6" s="112"/>
@@ -3843,15 +3788,23 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
     <mergeCell ref="E26:J26"/>
@@ -3867,23 +3820,15 @@
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
     <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E43:J43"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -4006,7 +3951,7 @@
       <c r="G5" s="41"/>
       <c r="H5" s="42"/>
       <c r="I5" s="122" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="J5" s="123"/>
     </row>
@@ -4049,7 +3994,7 @@
     <row r="9" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="40"/>
       <c r="B9" s="41" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="C9" s="41"/>
       <c r="D9" s="41"/>
@@ -4144,7 +4089,7 @@
       <c r="G16" s="41"/>
       <c r="H16" s="43"/>
       <c r="I16" s="118" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="J16" s="119"/>
     </row>
@@ -4451,7 +4396,7 @@
     <row r="42" spans="1:10" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="40"/>
       <c r="B42" s="41" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C42" s="41"/>
       <c r="D42" s="41"/>
@@ -4737,10 +4682,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R59"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A25" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4848,19 +4793,19 @@
         <v>44</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="89" t="s">
+        <v>218</v>
+      </c>
+      <c r="D4" s="89" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" s="24" t="s">
         <v>222</v>
-      </c>
-      <c r="D4" s="89" t="s">
-        <v>223</v>
-      </c>
-      <c r="E4" s="24" t="s">
-        <v>225</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>226</v>
       </c>
       <c r="G4" s="24" t="s">
         <v>56</v>
@@ -4904,7 +4849,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="97" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C5" s="97">
         <v>51</v>
@@ -4913,7 +4858,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="97" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="F5" s="97" t="s">
         <v>143</v>
@@ -4936,7 +4881,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" s="98"/>
       <c r="D6" s="98">
@@ -4978,7 +4923,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C7" s="98"/>
       <c r="D7" s="98">
@@ -5018,7 +4963,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C8" s="98"/>
       <c r="D8" s="98">
@@ -5056,7 +5001,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C9" s="98"/>
       <c r="D9" s="98">
@@ -5094,7 +5039,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C10" s="98"/>
       <c r="D10" s="98">
@@ -5132,7 +5077,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C11" s="98"/>
       <c r="D11" s="98">
@@ -5170,7 +5115,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C12" s="98"/>
       <c r="D12" s="98">
@@ -5208,7 +5153,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C13" s="98"/>
       <c r="D13" s="98">
@@ -5246,7 +5191,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C14" s="98"/>
       <c r="D14" s="98">
@@ -5284,7 +5229,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C15" s="98"/>
       <c r="D15" s="98">
@@ -5322,7 +5267,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C16" s="98"/>
       <c r="D16" s="98">
@@ -5360,7 +5305,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C17" s="98"/>
       <c r="D17" s="98">
@@ -5398,7 +5343,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C18" s="98"/>
       <c r="D18" s="98">
@@ -5436,7 +5381,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C19" s="98"/>
       <c r="D19" s="98">
@@ -5476,7 +5421,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C20" s="98"/>
       <c r="D20" s="98">
@@ -5486,7 +5431,7 @@
         <v>114</v>
       </c>
       <c r="F20" s="88" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G20" s="62"/>
       <c r="H20" s="37" t="s">
@@ -5512,7 +5457,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C21" s="98"/>
       <c r="D21" s="98">
@@ -5522,7 +5467,7 @@
         <v>121</v>
       </c>
       <c r="F21" s="88" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="G21" s="56"/>
       <c r="H21" s="37" t="s">
@@ -5548,7 +5493,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C22" s="98"/>
       <c r="D22" s="98">
@@ -5558,7 +5503,7 @@
         <v>122</v>
       </c>
       <c r="F22" s="88" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G22" s="56"/>
       <c r="H22" s="37" t="s">
@@ -5582,7 +5527,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C23" s="98"/>
       <c r="D23" s="98">
@@ -5592,7 +5537,7 @@
         <v>115</v>
       </c>
       <c r="F23" s="88" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G23" s="56"/>
       <c r="H23" s="37" t="s">
@@ -5618,7 +5563,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="98" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C24" s="98"/>
       <c r="D24" s="98">
@@ -5653,214 +5598,166 @@
         <v>169</v>
       </c>
     </row>
-    <row r="25" spans="1:18" s="33" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="97">
+    <row r="25" spans="1:18" s="33" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="98">
         <v>21</v>
       </c>
       <c r="B25" s="97" t="s">
-        <v>219</v>
-      </c>
-      <c r="C25" s="97"/>
+        <v>217</v>
+      </c>
+      <c r="C25" s="97">
+        <v>51</v>
+      </c>
       <c r="D25" s="97">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E25" s="99" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F25" s="99" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G25" s="99" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H25" s="93" t="s">
         <v>123</v>
       </c>
       <c r="I25" s="93" t="s">
-        <v>231</v>
+        <v>45</v>
       </c>
       <c r="J25" s="93"/>
       <c r="K25" s="100"/>
       <c r="L25" s="100"/>
-      <c r="M25" s="101"/>
+      <c r="M25" s="101" t="s">
+        <v>119</v>
+      </c>
       <c r="N25" s="101"/>
       <c r="O25" s="93"/>
       <c r="P25" s="99"/>
       <c r="Q25" s="99"/>
       <c r="R25" s="99" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" s="33" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="102">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" s="33" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="32">
         <v>22</v>
       </c>
       <c r="B26" s="97" t="s">
-        <v>219</v>
-      </c>
-      <c r="C26" s="97"/>
+        <v>217</v>
+      </c>
+      <c r="C26" s="97">
+        <v>51</v>
+      </c>
       <c r="D26" s="97">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E26" s="99" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F26" s="99" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="G26" s="99" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="H26" s="93" t="s">
         <v>123</v>
       </c>
       <c r="I26" s="93" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="J26" s="93"/>
       <c r="K26" s="100"/>
       <c r="L26" s="100"/>
-      <c r="M26" s="101"/>
+      <c r="M26" s="101" t="s">
+        <v>119</v>
+      </c>
       <c r="N26" s="101"/>
       <c r="O26" s="93"/>
       <c r="P26" s="99"/>
       <c r="Q26" s="99"/>
       <c r="R26" s="99" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" s="33" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="97">
-        <v>23</v>
-      </c>
-      <c r="B27" s="97" t="s">
-        <v>219</v>
-      </c>
-      <c r="C27" s="97">
-        <v>51</v>
-      </c>
-      <c r="D27" s="97">
-        <v>22</v>
-      </c>
-      <c r="E27" s="99" t="s">
-        <v>214</v>
-      </c>
-      <c r="F27" s="99" t="s">
-        <v>215</v>
-      </c>
-      <c r="G27" s="99" t="s">
-        <v>215</v>
-      </c>
-      <c r="H27" s="93" t="s">
-        <v>123</v>
-      </c>
-      <c r="I27" s="93" t="s">
-        <v>45</v>
-      </c>
-      <c r="J27" s="93"/>
-      <c r="K27" s="100"/>
-      <c r="L27" s="100"/>
-      <c r="M27" s="101" t="s">
-        <v>119</v>
-      </c>
-      <c r="N27" s="101"/>
-      <c r="O27" s="93"/>
-      <c r="P27" s="99"/>
-      <c r="Q27" s="99"/>
-      <c r="R27" s="99" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" s="33" customFormat="1" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="102">
-        <v>24</v>
-      </c>
-      <c r="B28" s="97" t="s">
-        <v>219</v>
-      </c>
-      <c r="C28" s="97">
-        <v>51</v>
-      </c>
-      <c r="D28" s="97">
-        <v>23</v>
-      </c>
-      <c r="E28" s="99" t="s">
-        <v>211</v>
-      </c>
-      <c r="F28" s="99" t="s">
-        <v>216</v>
-      </c>
-      <c r="G28" s="99" t="s">
-        <v>216</v>
-      </c>
-      <c r="H28" s="93" t="s">
-        <v>123</v>
-      </c>
-      <c r="I28" s="93" t="s">
-        <v>231</v>
-      </c>
-      <c r="J28" s="93"/>
-      <c r="K28" s="100"/>
-      <c r="L28" s="100"/>
-      <c r="M28" s="101" t="s">
-        <v>119</v>
-      </c>
-      <c r="N28" s="101"/>
-      <c r="O28" s="93"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="99"/>
-      <c r="R28" s="99" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" s="33" customFormat="1" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="97">
-        <v>25</v>
-      </c>
-      <c r="B29" s="97" t="s">
-        <v>219</v>
-      </c>
-      <c r="C29" s="97"/>
-      <c r="D29" s="97">
-        <v>24</v>
-      </c>
-      <c r="E29" s="99" t="s">
-        <v>220</v>
-      </c>
-      <c r="F29" s="99" t="s">
-        <v>221</v>
-      </c>
-      <c r="G29" s="99" t="s">
-        <v>221</v>
-      </c>
-      <c r="H29" s="93" t="s">
-        <v>125</v>
-      </c>
-      <c r="I29" s="93" t="s">
-        <v>45</v>
-      </c>
-      <c r="J29" s="93"/>
-      <c r="K29" s="100"/>
-      <c r="L29" s="100"/>
-      <c r="M29" s="101"/>
-      <c r="N29" s="101"/>
-      <c r="O29" s="93"/>
-      <c r="P29" s="99"/>
-      <c r="Q29" s="99"/>
-      <c r="R29" s="103" t="s">
-        <v>232</v>
-      </c>
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="32">
+        <v>26</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="37"/>
+      <c r="K27" s="58"/>
+      <c r="L27" s="58"/>
+      <c r="M27" s="57"/>
+      <c r="N27" s="57"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="56"/>
+      <c r="Q27" s="56"/>
+      <c r="R27" s="61"/>
+    </row>
+    <row r="28" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="98">
+        <v>27</v>
+      </c>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="55"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
+      <c r="K28" s="58"/>
+      <c r="L28" s="58"/>
+      <c r="M28" s="57"/>
+      <c r="N28" s="57"/>
+      <c r="O28" s="37"/>
+      <c r="P28" s="56"/>
+      <c r="Q28" s="56"/>
+      <c r="R28" s="56"/>
+    </row>
+    <row r="29" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="32">
+        <v>28</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
+      <c r="K29" s="58"/>
+      <c r="L29" s="58"/>
+      <c r="M29" s="57"/>
+      <c r="N29" s="57"/>
+      <c r="O29" s="37"/>
+      <c r="P29" s="56"/>
+      <c r="Q29" s="56"/>
+      <c r="R29" s="56"/>
     </row>
     <row r="30" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="32">
-        <v>26</v>
+      <c r="A30" s="98">
+        <v>29</v>
       </c>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
       <c r="D30" s="32"/>
       <c r="E30" s="55"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="68"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="62"/>
       <c r="H30" s="37"/>
       <c r="I30" s="37"/>
       <c r="J30" s="37"/>
@@ -5869,20 +5766,20 @@
       <c r="M30" s="57"/>
       <c r="N30" s="57"/>
       <c r="O30" s="37"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
+      <c r="P30" s="61"/>
+      <c r="Q30" s="61"/>
       <c r="R30" s="61"/>
     </row>
     <row r="31" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="98">
-        <v>27</v>
+      <c r="A31" s="32">
+        <v>30</v>
       </c>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
       <c r="D31" s="32"/>
       <c r="E31" s="55"/>
       <c r="F31" s="61"/>
-      <c r="G31" s="62"/>
+      <c r="G31" s="61"/>
       <c r="H31" s="37"/>
       <c r="I31" s="37"/>
       <c r="J31" s="37"/>
@@ -5891,20 +5788,20 @@
       <c r="M31" s="57"/>
       <c r="N31" s="57"/>
       <c r="O31" s="37"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
+      <c r="P31" s="61"/>
+      <c r="Q31" s="61"/>
+      <c r="R31" s="61"/>
     </row>
     <row r="32" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="32">
-        <v>28</v>
+      <c r="A32" s="98">
+        <v>31</v>
       </c>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
       <c r="D32" s="32"/>
       <c r="E32" s="55"/>
       <c r="F32" s="61"/>
-      <c r="G32" s="62"/>
+      <c r="G32" s="61"/>
       <c r="H32" s="37"/>
       <c r="I32" s="37"/>
       <c r="J32" s="37"/>
@@ -5913,20 +5810,20 @@
       <c r="M32" s="57"/>
       <c r="N32" s="57"/>
       <c r="O32" s="37"/>
-      <c r="P32" s="56"/>
-      <c r="Q32" s="56"/>
-      <c r="R32" s="56"/>
+      <c r="P32" s="61"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="62"/>
     </row>
     <row r="33" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="98">
-        <v>29</v>
+      <c r="A33" s="32">
+        <v>32</v>
       </c>
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
       <c r="D33" s="32"/>
       <c r="E33" s="55"/>
       <c r="F33" s="61"/>
-      <c r="G33" s="62"/>
+      <c r="G33" s="61"/>
       <c r="H33" s="37"/>
       <c r="I33" s="37"/>
       <c r="J33" s="37"/>
@@ -5940,15 +5837,15 @@
       <c r="R33" s="61"/>
     </row>
     <row r="34" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="32">
-        <v>30</v>
+      <c r="A34" s="98">
+        <v>33</v>
       </c>
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
       <c r="D34" s="32"/>
       <c r="E34" s="55"/>
       <c r="F34" s="61"/>
-      <c r="G34" s="61"/>
+      <c r="G34" s="56"/>
       <c r="H34" s="37"/>
       <c r="I34" s="37"/>
       <c r="J34" s="37"/>
@@ -5957,20 +5854,20 @@
       <c r="M34" s="57"/>
       <c r="N34" s="57"/>
       <c r="O34" s="37"/>
-      <c r="P34" s="61"/>
-      <c r="Q34" s="61"/>
+      <c r="P34" s="56"/>
+      <c r="Q34" s="56"/>
       <c r="R34" s="61"/>
     </row>
     <row r="35" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="98">
-        <v>31</v>
+      <c r="A35" s="32">
+        <v>34</v>
       </c>
       <c r="B35" s="32"/>
       <c r="C35" s="32"/>
       <c r="D35" s="32"/>
       <c r="E35" s="55"/>
       <c r="F35" s="61"/>
-      <c r="G35" s="61"/>
+      <c r="G35" s="56"/>
       <c r="H35" s="37"/>
       <c r="I35" s="37"/>
       <c r="J35" s="37"/>
@@ -5979,20 +5876,20 @@
       <c r="M35" s="57"/>
       <c r="N35" s="57"/>
       <c r="O35" s="37"/>
-      <c r="P35" s="61"/>
-      <c r="Q35" s="61"/>
-      <c r="R35" s="62"/>
+      <c r="P35" s="56"/>
+      <c r="Q35" s="56"/>
+      <c r="R35" s="61"/>
     </row>
     <row r="36" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="32">
-        <v>32</v>
+      <c r="A36" s="98">
+        <v>35</v>
       </c>
       <c r="B36" s="32"/>
       <c r="C36" s="32"/>
       <c r="D36" s="32"/>
       <c r="E36" s="55"/>
       <c r="F36" s="61"/>
-      <c r="G36" s="61"/>
+      <c r="G36" s="56"/>
       <c r="H36" s="37"/>
       <c r="I36" s="37"/>
       <c r="J36" s="37"/>
@@ -6001,19 +5898,19 @@
       <c r="M36" s="57"/>
       <c r="N36" s="57"/>
       <c r="O36" s="37"/>
-      <c r="P36" s="61"/>
-      <c r="Q36" s="61"/>
+      <c r="P36" s="56"/>
+      <c r="Q36" s="56"/>
       <c r="R36" s="61"/>
     </row>
     <row r="37" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="98">
-        <v>33</v>
+      <c r="A37" s="32">
+        <v>36</v>
       </c>
       <c r="B37" s="32"/>
       <c r="C37" s="32"/>
       <c r="D37" s="32"/>
       <c r="E37" s="55"/>
-      <c r="F37" s="61"/>
+      <c r="F37" s="56"/>
       <c r="G37" s="56"/>
       <c r="H37" s="37"/>
       <c r="I37" s="37"/>
@@ -6025,17 +5922,17 @@
       <c r="O37" s="37"/>
       <c r="P37" s="56"/>
       <c r="Q37" s="56"/>
-      <c r="R37" s="61"/>
+      <c r="R37" s="56"/>
     </row>
     <row r="38" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="32">
-        <v>34</v>
+      <c r="A38" s="98">
+        <v>37</v>
       </c>
       <c r="B38" s="32"/>
       <c r="C38" s="32"/>
       <c r="D38" s="32"/>
       <c r="E38" s="55"/>
-      <c r="F38" s="61"/>
+      <c r="F38" s="56"/>
       <c r="G38" s="56"/>
       <c r="H38" s="37"/>
       <c r="I38" s="37"/>
@@ -6047,17 +5944,17 @@
       <c r="O38" s="37"/>
       <c r="P38" s="56"/>
       <c r="Q38" s="56"/>
-      <c r="R38" s="61"/>
+      <c r="R38" s="56"/>
     </row>
     <row r="39" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="98">
-        <v>35</v>
+      <c r="A39" s="32">
+        <v>38</v>
       </c>
       <c r="B39" s="32"/>
       <c r="C39" s="32"/>
       <c r="D39" s="32"/>
       <c r="E39" s="55"/>
-      <c r="F39" s="61"/>
+      <c r="F39" s="56"/>
       <c r="G39" s="56"/>
       <c r="H39" s="37"/>
       <c r="I39" s="37"/>
@@ -6069,11 +5966,11 @@
       <c r="O39" s="37"/>
       <c r="P39" s="56"/>
       <c r="Q39" s="56"/>
-      <c r="R39" s="61"/>
+      <c r="R39" s="56"/>
     </row>
     <row r="40" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="32">
-        <v>36</v>
+      <c r="A40" s="98">
+        <v>39</v>
       </c>
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
@@ -6094,8 +5991,8 @@
       <c r="R40" s="56"/>
     </row>
     <row r="41" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="98">
-        <v>37</v>
+      <c r="A41" s="32">
+        <v>40</v>
       </c>
       <c r="B41" s="32"/>
       <c r="C41" s="32"/>
@@ -6116,8 +6013,8 @@
       <c r="R41" s="56"/>
     </row>
     <row r="42" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="32">
-        <v>38</v>
+      <c r="A42" s="98">
+        <v>41</v>
       </c>
       <c r="B42" s="32"/>
       <c r="C42" s="32"/>
@@ -6137,9 +6034,9 @@
       <c r="Q42" s="56"/>
       <c r="R42" s="56"/>
     </row>
-    <row r="43" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="98">
-        <v>39</v>
+    <row r="43" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="32">
+        <v>42</v>
       </c>
       <c r="B43" s="32"/>
       <c r="C43" s="32"/>
@@ -6159,9 +6056,9 @@
       <c r="Q43" s="56"/>
       <c r="R43" s="56"/>
     </row>
-    <row r="44" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="32">
-        <v>40</v>
+    <row r="44" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="98">
+        <v>43</v>
       </c>
       <c r="B44" s="32"/>
       <c r="C44" s="32"/>
@@ -6181,9 +6078,9 @@
       <c r="Q44" s="56"/>
       <c r="R44" s="56"/>
     </row>
-    <row r="45" spans="1:18" s="33" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="98">
-        <v>41</v>
+    <row r="45" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="32">
+        <v>44</v>
       </c>
       <c r="B45" s="32"/>
       <c r="C45" s="32"/>
@@ -6204,8 +6101,8 @@
       <c r="R45" s="56"/>
     </row>
     <row r="46" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="32">
-        <v>42</v>
+      <c r="A46" s="98">
+        <v>45</v>
       </c>
       <c r="B46" s="32"/>
       <c r="C46" s="32"/>
@@ -6226,8 +6123,8 @@
       <c r="R46" s="56"/>
     </row>
     <row r="47" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="98">
-        <v>43</v>
+      <c r="A47" s="32">
+        <v>46</v>
       </c>
       <c r="B47" s="32"/>
       <c r="C47" s="32"/>
@@ -6248,8 +6145,8 @@
       <c r="R47" s="56"/>
     </row>
     <row r="48" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="32">
-        <v>44</v>
+      <c r="A48" s="98">
+        <v>47</v>
       </c>
       <c r="B48" s="32"/>
       <c r="C48" s="32"/>
@@ -6270,8 +6167,8 @@
       <c r="R48" s="56"/>
     </row>
     <row r="49" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="98">
-        <v>45</v>
+      <c r="A49" s="32">
+        <v>48</v>
       </c>
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
@@ -6292,8 +6189,8 @@
       <c r="R49" s="56"/>
     </row>
     <row r="50" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="32">
-        <v>46</v>
+      <c r="A50" s="98">
+        <v>49</v>
       </c>
       <c r="B50" s="32"/>
       <c r="C50" s="32"/>
@@ -6314,8 +6211,8 @@
       <c r="R50" s="56"/>
     </row>
     <row r="51" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="98">
-        <v>47</v>
+      <c r="A51" s="32">
+        <v>50</v>
       </c>
       <c r="B51" s="32"/>
       <c r="C51" s="32"/>
@@ -6336,8 +6233,8 @@
       <c r="R51" s="56"/>
     </row>
     <row r="52" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="32">
-        <v>48</v>
+      <c r="A52" s="98">
+        <v>51</v>
       </c>
       <c r="B52" s="32"/>
       <c r="C52" s="32"/>
@@ -6358,8 +6255,8 @@
       <c r="R52" s="56"/>
     </row>
     <row r="53" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="98">
-        <v>49</v>
+      <c r="A53" s="32">
+        <v>52</v>
       </c>
       <c r="B53" s="32"/>
       <c r="C53" s="32"/>
@@ -6380,8 +6277,8 @@
       <c r="R53" s="56"/>
     </row>
     <row r="54" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="32">
-        <v>50</v>
+      <c r="A54" s="98">
+        <v>53</v>
       </c>
       <c r="B54" s="32"/>
       <c r="C54" s="32"/>
@@ -6402,8 +6299,8 @@
       <c r="R54" s="56"/>
     </row>
     <row r="55" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="98">
-        <v>51</v>
+      <c r="A55" s="32">
+        <v>54</v>
       </c>
       <c r="B55" s="32"/>
       <c r="C55" s="32"/>
@@ -6424,8 +6321,8 @@
       <c r="R55" s="56"/>
     </row>
     <row r="56" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="32">
-        <v>52</v>
+      <c r="A56" s="98">
+        <v>55</v>
       </c>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
@@ -6445,72 +6342,6 @@
       <c r="Q56" s="56"/>
       <c r="R56" s="56"/>
     </row>
-    <row r="57" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="98">
-        <v>53</v>
-      </c>
-      <c r="B57" s="32"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="56"/>
-      <c r="G57" s="56"/>
-      <c r="H57" s="37"/>
-      <c r="I57" s="37"/>
-      <c r="J57" s="37"/>
-      <c r="K57" s="58"/>
-      <c r="L57" s="58"/>
-      <c r="M57" s="57"/>
-      <c r="N57" s="57"/>
-      <c r="O57" s="37"/>
-      <c r="P57" s="56"/>
-      <c r="Q57" s="56"/>
-      <c r="R57" s="56"/>
-    </row>
-    <row r="58" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="32">
-        <v>54</v>
-      </c>
-      <c r="B58" s="32"/>
-      <c r="C58" s="32"/>
-      <c r="D58" s="32"/>
-      <c r="E58" s="55"/>
-      <c r="F58" s="56"/>
-      <c r="G58" s="56"/>
-      <c r="H58" s="37"/>
-      <c r="I58" s="37"/>
-      <c r="J58" s="37"/>
-      <c r="K58" s="58"/>
-      <c r="L58" s="58"/>
-      <c r="M58" s="57"/>
-      <c r="N58" s="57"/>
-      <c r="O58" s="37"/>
-      <c r="P58" s="56"/>
-      <c r="Q58" s="56"/>
-      <c r="R58" s="56"/>
-    </row>
-    <row r="59" spans="1:18" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="98">
-        <v>55</v>
-      </c>
-      <c r="B59" s="32"/>
-      <c r="C59" s="32"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="55"/>
-      <c r="F59" s="56"/>
-      <c r="G59" s="56"/>
-      <c r="H59" s="37"/>
-      <c r="I59" s="37"/>
-      <c r="J59" s="37"/>
-      <c r="K59" s="58"/>
-      <c r="L59" s="58"/>
-      <c r="M59" s="57"/>
-      <c r="N59" s="57"/>
-      <c r="O59" s="37"/>
-      <c r="P59" s="56"/>
-      <c r="Q59" s="56"/>
-      <c r="R59" s="56"/>
-    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A1:F2"/>
@@ -6520,20 +6351,20 @@
     <mergeCell ref="K2:N2"/>
   </mergeCells>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6">
+      <formula1>"Caption,Textbox,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid,Image,Link,Other"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J56">
       <formula1>"Text, Number, DateTime, Boolean"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6:N59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6:N56">
       <formula1>"   ,l"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H56">
       <formula1>"Textbox,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid,Image,Link,Other"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I59">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I56">
       <formula1>"I,O,I/O"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6">
-      <formula1>"Caption,Textbox,RichTextbox,Label,ComboBox,CheckBox,RadioButton,Button,DataGrid,Image,Link,Other"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
@@ -6657,7 +6488,7 @@
         <v>44</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="24" t="s">
         <v>55</v>
@@ -6707,7 +6538,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C5" s="61"/>
       <c r="D5" s="80" t="s">
@@ -6743,7 +6574,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" s="61"/>
       <c r="D6" s="80" t="s">
@@ -6779,7 +6610,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="68" t="s">
@@ -7795,10 +7626,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P54"/>
+  <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A43" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A33" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7901,10 +7732,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="90" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C4" s="106" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="D4" s="36" t="s">
         <v>55</v>
@@ -7939,7 +7770,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C5" s="32"/>
       <c r="D5" s="80" t="s">
@@ -7953,13 +7784,13 @@
       <c r="H5" s="118" t="s">
         <v>173</v>
       </c>
-      <c r="I5" s="142"/>
-      <c r="J5" s="142"/>
-      <c r="K5" s="143"/>
-      <c r="L5" s="136" t="s">
+      <c r="I5" s="136"/>
+      <c r="J5" s="136"/>
+      <c r="K5" s="137"/>
+      <c r="L5" s="147" t="s">
         <v>174</v>
       </c>
-      <c r="M5" s="136" t="s">
+      <c r="M5" s="147" t="s">
         <v>188</v>
       </c>
       <c r="N5" s="37"/>
@@ -7971,7 +7802,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C6" s="32"/>
       <c r="D6" s="68" t="s">
@@ -7982,12 +7813,12 @@
       </c>
       <c r="F6" s="59"/>
       <c r="G6" s="37"/>
-      <c r="H6" s="144"/>
-      <c r="I6" s="145"/>
-      <c r="J6" s="145"/>
-      <c r="K6" s="146"/>
-      <c r="L6" s="137"/>
-      <c r="M6" s="137"/>
+      <c r="H6" s="138"/>
+      <c r="I6" s="139"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="148"/>
+      <c r="M6" s="148"/>
       <c r="N6" s="37"/>
       <c r="O6" s="60"/>
       <c r="P6" s="60"/>
@@ -7997,7 +7828,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C7" s="32"/>
       <c r="D7" s="68" t="s">
@@ -8008,12 +7839,12 @@
       </c>
       <c r="F7" s="59"/>
       <c r="G7" s="37"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="145"/>
-      <c r="J7" s="145"/>
-      <c r="K7" s="146"/>
-      <c r="L7" s="137"/>
-      <c r="M7" s="137"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="148"/>
+      <c r="M7" s="148"/>
       <c r="N7" s="37"/>
       <c r="O7" s="60"/>
       <c r="P7" s="60"/>
@@ -8023,7 +7854,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C8" s="32"/>
       <c r="D8" s="68" t="s">
@@ -8034,12 +7865,12 @@
       </c>
       <c r="F8" s="59"/>
       <c r="G8" s="37"/>
-      <c r="H8" s="144"/>
-      <c r="I8" s="145"/>
-      <c r="J8" s="145"/>
-      <c r="K8" s="146"/>
-      <c r="L8" s="137"/>
-      <c r="M8" s="137"/>
+      <c r="H8" s="138"/>
+      <c r="I8" s="139"/>
+      <c r="J8" s="139"/>
+      <c r="K8" s="140"/>
+      <c r="L8" s="148"/>
+      <c r="M8" s="148"/>
       <c r="N8" s="37"/>
       <c r="O8" s="60"/>
       <c r="P8" s="60"/>
@@ -8049,7 +7880,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="68" t="s">
@@ -8060,12 +7891,12 @@
       </c>
       <c r="F9" s="59"/>
       <c r="G9" s="37"/>
-      <c r="H9" s="144"/>
-      <c r="I9" s="145"/>
-      <c r="J9" s="145"/>
-      <c r="K9" s="146"/>
-      <c r="L9" s="137"/>
-      <c r="M9" s="137"/>
+      <c r="H9" s="138"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="139"/>
+      <c r="K9" s="140"/>
+      <c r="L9" s="148"/>
+      <c r="M9" s="148"/>
       <c r="N9" s="37"/>
       <c r="O9" s="60"/>
       <c r="P9" s="60"/>
@@ -8075,7 +7906,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C10" s="32"/>
       <c r="D10" s="68" t="s">
@@ -8086,12 +7917,12 @@
       </c>
       <c r="F10" s="59"/>
       <c r="G10" s="37"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="145"/>
-      <c r="J10" s="145"/>
-      <c r="K10" s="146"/>
-      <c r="L10" s="137"/>
-      <c r="M10" s="137"/>
+      <c r="H10" s="138"/>
+      <c r="I10" s="139"/>
+      <c r="J10" s="139"/>
+      <c r="K10" s="140"/>
+      <c r="L10" s="148"/>
+      <c r="M10" s="148"/>
       <c r="N10" s="37"/>
       <c r="O10" s="60"/>
       <c r="P10" s="60"/>
@@ -8101,7 +7932,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C11" s="32"/>
       <c r="D11" s="68" t="s">
@@ -8112,12 +7943,12 @@
       </c>
       <c r="F11" s="59"/>
       <c r="G11" s="37"/>
-      <c r="H11" s="144"/>
-      <c r="I11" s="145"/>
-      <c r="J11" s="145"/>
-      <c r="K11" s="146"/>
-      <c r="L11" s="137"/>
-      <c r="M11" s="137"/>
+      <c r="H11" s="138"/>
+      <c r="I11" s="139"/>
+      <c r="J11" s="139"/>
+      <c r="K11" s="140"/>
+      <c r="L11" s="148"/>
+      <c r="M11" s="148"/>
       <c r="N11" s="37"/>
       <c r="O11" s="60"/>
       <c r="P11" s="60"/>
@@ -8127,7 +7958,7 @@
         <v>8</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C12" s="32"/>
       <c r="D12" s="68" t="s">
@@ -8138,12 +7969,12 @@
       </c>
       <c r="F12" s="59"/>
       <c r="G12" s="37"/>
-      <c r="H12" s="144"/>
-      <c r="I12" s="145"/>
-      <c r="J12" s="145"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="137"/>
-      <c r="M12" s="137"/>
+      <c r="H12" s="138"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="140"/>
+      <c r="L12" s="148"/>
+      <c r="M12" s="148"/>
       <c r="N12" s="37"/>
       <c r="O12" s="60"/>
       <c r="P12" s="60"/>
@@ -8153,7 +7984,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C13" s="32"/>
       <c r="D13" s="68" t="s">
@@ -8164,12 +7995,12 @@
       </c>
       <c r="F13" s="59"/>
       <c r="G13" s="37"/>
-      <c r="H13" s="144"/>
-      <c r="I13" s="145"/>
-      <c r="J13" s="145"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="137"/>
-      <c r="M13" s="137"/>
+      <c r="H13" s="138"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="139"/>
+      <c r="K13" s="140"/>
+      <c r="L13" s="148"/>
+      <c r="M13" s="148"/>
       <c r="N13" s="37"/>
       <c r="O13" s="60"/>
       <c r="P13" s="60"/>
@@ -8179,7 +8010,7 @@
         <v>10</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C14" s="32"/>
       <c r="D14" s="68" t="s">
@@ -8190,12 +8021,12 @@
       </c>
       <c r="F14" s="59"/>
       <c r="G14" s="37"/>
-      <c r="H14" s="144"/>
-      <c r="I14" s="145"/>
-      <c r="J14" s="145"/>
-      <c r="K14" s="146"/>
-      <c r="L14" s="137"/>
-      <c r="M14" s="137"/>
+      <c r="H14" s="138"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="139"/>
+      <c r="K14" s="140"/>
+      <c r="L14" s="148"/>
+      <c r="M14" s="148"/>
       <c r="N14" s="37"/>
       <c r="O14" s="60"/>
       <c r="P14" s="60"/>
@@ -8205,7 +8036,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C15" s="32"/>
       <c r="D15" s="68" t="s">
@@ -8216,12 +8047,12 @@
       </c>
       <c r="F15" s="59"/>
       <c r="G15" s="37"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="145"/>
-      <c r="J15" s="145"/>
-      <c r="K15" s="146"/>
-      <c r="L15" s="137"/>
-      <c r="M15" s="137"/>
+      <c r="H15" s="138"/>
+      <c r="I15" s="139"/>
+      <c r="J15" s="139"/>
+      <c r="K15" s="140"/>
+      <c r="L15" s="148"/>
+      <c r="M15" s="148"/>
       <c r="N15" s="37"/>
       <c r="O15" s="60"/>
       <c r="P15" s="60"/>
@@ -8231,7 +8062,7 @@
         <v>12</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C16" s="32"/>
       <c r="D16" s="68" t="s">
@@ -8242,12 +8073,12 @@
       </c>
       <c r="F16" s="59"/>
       <c r="G16" s="37"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="145"/>
-      <c r="J16" s="145"/>
-      <c r="K16" s="146"/>
-      <c r="L16" s="137"/>
-      <c r="M16" s="137"/>
+      <c r="H16" s="138"/>
+      <c r="I16" s="139"/>
+      <c r="J16" s="139"/>
+      <c r="K16" s="140"/>
+      <c r="L16" s="148"/>
+      <c r="M16" s="148"/>
       <c r="N16" s="37"/>
       <c r="O16" s="60"/>
       <c r="P16" s="60"/>
@@ -8257,7 +8088,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C17" s="32"/>
       <c r="D17" s="68" t="s">
@@ -8268,12 +8099,12 @@
       </c>
       <c r="F17" s="59"/>
       <c r="G17" s="37"/>
-      <c r="H17" s="162"/>
-      <c r="I17" s="163"/>
-      <c r="J17" s="163"/>
-      <c r="K17" s="164"/>
-      <c r="L17" s="138"/>
-      <c r="M17" s="138"/>
+      <c r="H17" s="141"/>
+      <c r="I17" s="142"/>
+      <c r="J17" s="142"/>
+      <c r="K17" s="143"/>
+      <c r="L17" s="149"/>
+      <c r="M17" s="149"/>
       <c r="N17" s="37"/>
       <c r="O17" s="60"/>
       <c r="P17" s="60"/>
@@ -8283,7 +8114,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C18" s="32"/>
       <c r="D18" s="68" t="s">
@@ -8294,12 +8125,12 @@
       </c>
       <c r="F18" s="59"/>
       <c r="G18" s="37"/>
-      <c r="H18" s="139" t="s">
+      <c r="H18" s="144" t="s">
         <v>206</v>
       </c>
-      <c r="I18" s="140"/>
-      <c r="J18" s="140"/>
-      <c r="K18" s="141"/>
+      <c r="I18" s="145"/>
+      <c r="J18" s="145"/>
+      <c r="K18" s="146"/>
       <c r="L18" s="86"/>
       <c r="M18" s="86"/>
       <c r="N18" s="80" t="s">
@@ -8313,7 +8144,7 @@
         <v>15</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C19" s="32"/>
       <c r="D19" s="68" t="s">
@@ -8324,12 +8155,12 @@
       </c>
       <c r="F19" s="59"/>
       <c r="G19" s="37"/>
-      <c r="H19" s="139" t="s">
+      <c r="H19" s="144" t="s">
         <v>207</v>
       </c>
-      <c r="I19" s="140"/>
-      <c r="J19" s="140"/>
-      <c r="K19" s="141"/>
+      <c r="I19" s="145"/>
+      <c r="J19" s="145"/>
+      <c r="K19" s="146"/>
       <c r="L19" s="86"/>
       <c r="M19" s="86"/>
       <c r="N19" s="80" t="s">
@@ -8343,7 +8174,7 @@
         <v>16</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C20" s="32"/>
       <c r="D20" s="68" t="s">
@@ -8354,12 +8185,12 @@
       </c>
       <c r="F20" s="59"/>
       <c r="G20" s="37"/>
-      <c r="H20" s="139" t="s">
+      <c r="H20" s="144" t="s">
         <v>208</v>
       </c>
-      <c r="I20" s="140"/>
-      <c r="J20" s="140"/>
-      <c r="K20" s="141"/>
+      <c r="I20" s="145"/>
+      <c r="J20" s="145"/>
+      <c r="K20" s="146"/>
       <c r="L20" s="87" t="s">
         <v>177</v>
       </c>
@@ -8377,7 +8208,7 @@
         <v>17</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C21" s="32"/>
       <c r="D21" s="68" t="s">
@@ -8388,12 +8219,12 @@
       </c>
       <c r="F21" s="59"/>
       <c r="G21" s="37"/>
-      <c r="H21" s="139" t="s">
+      <c r="H21" s="144" t="s">
         <v>209</v>
       </c>
-      <c r="I21" s="140"/>
-      <c r="J21" s="140"/>
-      <c r="K21" s="141"/>
+      <c r="I21" s="145"/>
+      <c r="J21" s="145"/>
+      <c r="K21" s="146"/>
       <c r="L21" s="87" t="s">
         <v>178</v>
       </c>
@@ -8411,7 +8242,7 @@
         <v>18</v>
       </c>
       <c r="B22" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C22" s="32"/>
       <c r="D22" s="80" t="s">
@@ -8425,9 +8256,9 @@
       <c r="H22" s="118" t="s">
         <v>175</v>
       </c>
-      <c r="I22" s="142"/>
-      <c r="J22" s="142"/>
-      <c r="K22" s="143"/>
+      <c r="I22" s="136"/>
+      <c r="J22" s="136"/>
+      <c r="K22" s="137"/>
       <c r="L22" s="81" t="s">
         <v>174</v>
       </c>
@@ -8443,7 +8274,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C23" s="32"/>
       <c r="D23" s="68" t="s">
@@ -8454,10 +8285,10 @@
       </c>
       <c r="F23" s="59"/>
       <c r="G23" s="37"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="145"/>
-      <c r="J23" s="145"/>
-      <c r="K23" s="146"/>
+      <c r="H23" s="138"/>
+      <c r="I23" s="139"/>
+      <c r="J23" s="139"/>
+      <c r="K23" s="140"/>
       <c r="L23" s="91" t="s">
         <v>176</v>
       </c>
@@ -8473,7 +8304,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C24" s="32"/>
       <c r="D24" s="68" t="s">
@@ -8484,10 +8315,10 @@
       </c>
       <c r="F24" s="59"/>
       <c r="G24" s="37"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="145"/>
-      <c r="J24" s="145"/>
-      <c r="K24" s="146"/>
+      <c r="H24" s="138"/>
+      <c r="I24" s="139"/>
+      <c r="J24" s="139"/>
+      <c r="K24" s="140"/>
       <c r="L24" s="91" t="s">
         <v>177</v>
       </c>
@@ -8503,7 +8334,7 @@
         <v>21</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C25" s="32"/>
       <c r="D25" s="68" t="s">
@@ -8514,10 +8345,10 @@
       </c>
       <c r="F25" s="59"/>
       <c r="G25" s="37"/>
-      <c r="H25" s="144"/>
-      <c r="I25" s="145"/>
-      <c r="J25" s="145"/>
-      <c r="K25" s="146"/>
+      <c r="H25" s="138"/>
+      <c r="I25" s="139"/>
+      <c r="J25" s="139"/>
+      <c r="K25" s="140"/>
       <c r="L25" s="91" t="s">
         <v>178</v>
       </c>
@@ -8533,7 +8364,7 @@
         <v>22</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C26" s="32"/>
       <c r="D26" s="68" t="s">
@@ -8544,10 +8375,10 @@
       </c>
       <c r="F26" s="59"/>
       <c r="G26" s="37"/>
-      <c r="H26" s="144"/>
-      <c r="I26" s="145"/>
-      <c r="J26" s="145"/>
-      <c r="K26" s="146"/>
+      <c r="H26" s="138"/>
+      <c r="I26" s="139"/>
+      <c r="J26" s="139"/>
+      <c r="K26" s="140"/>
       <c r="L26" s="91" t="s">
         <v>179</v>
       </c>
@@ -8563,7 +8394,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C27" s="32"/>
       <c r="D27" s="68" t="s">
@@ -8574,10 +8405,10 @@
       </c>
       <c r="F27" s="59"/>
       <c r="G27" s="37"/>
-      <c r="H27" s="144"/>
-      <c r="I27" s="145"/>
-      <c r="J27" s="145"/>
-      <c r="K27" s="146"/>
+      <c r="H27" s="138"/>
+      <c r="I27" s="139"/>
+      <c r="J27" s="139"/>
+      <c r="K27" s="140"/>
       <c r="L27" s="91" t="s">
         <v>180</v>
       </c>
@@ -8593,7 +8424,7 @@
         <v>24</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C28" s="32"/>
       <c r="D28" s="68" t="s">
@@ -8604,10 +8435,10 @@
       </c>
       <c r="F28" s="59"/>
       <c r="G28" s="37"/>
-      <c r="H28" s="144"/>
-      <c r="I28" s="145"/>
-      <c r="J28" s="145"/>
-      <c r="K28" s="146"/>
+      <c r="H28" s="138"/>
+      <c r="I28" s="139"/>
+      <c r="J28" s="139"/>
+      <c r="K28" s="140"/>
       <c r="L28" s="91" t="s">
         <v>181</v>
       </c>
@@ -8623,7 +8454,7 @@
         <v>25</v>
       </c>
       <c r="B29" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C29" s="32"/>
       <c r="D29" s="68" t="s">
@@ -8634,10 +8465,10 @@
       </c>
       <c r="F29" s="59"/>
       <c r="G29" s="37"/>
-      <c r="H29" s="144"/>
-      <c r="I29" s="145"/>
-      <c r="J29" s="145"/>
-      <c r="K29" s="146"/>
+      <c r="H29" s="138"/>
+      <c r="I29" s="139"/>
+      <c r="J29" s="139"/>
+      <c r="K29" s="140"/>
       <c r="L29" s="91" t="s">
         <v>182</v>
       </c>
@@ -8653,7 +8484,7 @@
         <v>26</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C30" s="32"/>
       <c r="D30" s="68" t="s">
@@ -8664,10 +8495,10 @@
       </c>
       <c r="F30" s="59"/>
       <c r="G30" s="37"/>
-      <c r="H30" s="144"/>
-      <c r="I30" s="145"/>
-      <c r="J30" s="145"/>
-      <c r="K30" s="146"/>
+      <c r="H30" s="138"/>
+      <c r="I30" s="139"/>
+      <c r="J30" s="139"/>
+      <c r="K30" s="140"/>
       <c r="L30" s="91" t="s">
         <v>183</v>
       </c>
@@ -8683,7 +8514,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C31" s="32"/>
       <c r="D31" s="68" t="s">
@@ -8694,10 +8525,10 @@
       </c>
       <c r="F31" s="59"/>
       <c r="G31" s="37"/>
-      <c r="H31" s="144"/>
-      <c r="I31" s="145"/>
-      <c r="J31" s="145"/>
-      <c r="K31" s="146"/>
+      <c r="H31" s="138"/>
+      <c r="I31" s="139"/>
+      <c r="J31" s="139"/>
+      <c r="K31" s="140"/>
       <c r="L31" s="91" t="s">
         <v>184</v>
       </c>
@@ -8713,7 +8544,7 @@
         <v>28</v>
       </c>
       <c r="B32" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C32" s="32"/>
       <c r="D32" s="68" t="s">
@@ -8724,10 +8555,10 @@
       </c>
       <c r="F32" s="59"/>
       <c r="G32" s="37"/>
-      <c r="H32" s="144"/>
-      <c r="I32" s="145"/>
-      <c r="J32" s="145"/>
-      <c r="K32" s="146"/>
+      <c r="H32" s="138"/>
+      <c r="I32" s="139"/>
+      <c r="J32" s="139"/>
+      <c r="K32" s="140"/>
       <c r="L32" s="91" t="s">
         <v>185</v>
       </c>
@@ -8743,7 +8574,7 @@
         <v>29</v>
       </c>
       <c r="B33" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C33" s="32"/>
       <c r="D33" s="68" t="s">
@@ -8754,10 +8585,10 @@
       </c>
       <c r="F33" s="59"/>
       <c r="G33" s="37"/>
-      <c r="H33" s="144"/>
-      <c r="I33" s="145"/>
-      <c r="J33" s="145"/>
-      <c r="K33" s="146"/>
+      <c r="H33" s="138"/>
+      <c r="I33" s="139"/>
+      <c r="J33" s="139"/>
+      <c r="K33" s="140"/>
       <c r="L33" s="91" t="s">
         <v>186</v>
       </c>
@@ -8773,7 +8604,7 @@
         <v>30</v>
       </c>
       <c r="B34" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C34" s="32"/>
       <c r="D34" s="68" t="s">
@@ -8805,7 +8636,7 @@
         <v>31</v>
       </c>
       <c r="B35" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C35" s="32"/>
       <c r="D35" s="68" t="s">
@@ -8835,7 +8666,7 @@
         <v>32</v>
       </c>
       <c r="B36" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C36" s="32"/>
       <c r="D36" s="68" t="s">
@@ -8865,7 +8696,7 @@
         <v>33</v>
       </c>
       <c r="B37" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C37" s="32"/>
       <c r="D37" s="68" t="s">
@@ -8895,7 +8726,7 @@
         <v>34</v>
       </c>
       <c r="B38" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C38" s="32"/>
       <c r="D38" s="68" t="s">
@@ -8925,7 +8756,7 @@
         <v>35</v>
       </c>
       <c r="B39" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C39" s="32"/>
       <c r="D39" s="68" t="s">
@@ -8955,7 +8786,7 @@
         <v>36</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C40" s="32"/>
       <c r="D40" s="68" t="s">
@@ -8985,7 +8816,7 @@
         <v>37</v>
       </c>
       <c r="B41" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C41" s="32"/>
       <c r="D41" s="68" t="s">
@@ -9015,7 +8846,7 @@
         <v>38</v>
       </c>
       <c r="B42" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C42" s="32"/>
       <c r="D42" s="68" t="s">
@@ -9045,7 +8876,7 @@
         <v>39</v>
       </c>
       <c r="B43" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C43" s="32"/>
       <c r="D43" s="68" t="s">
@@ -9075,7 +8906,7 @@
         <v>40</v>
       </c>
       <c r="B44" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C44" s="32"/>
       <c r="D44" s="68" t="s">
@@ -9105,7 +8936,7 @@
         <v>41</v>
       </c>
       <c r="B45" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C45" s="32"/>
       <c r="D45" s="68" t="s">
@@ -9154,134 +8985,102 @@
       <c r="O46" s="60"/>
       <c r="P46" s="60"/>
     </row>
-    <row r="47" spans="1:16" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="102">
+    <row r="47" spans="1:16" s="33" customFormat="1" ht="168.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="32">
         <v>43</v>
       </c>
       <c r="B47" s="102" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C47" s="102">
         <v>51</v>
       </c>
       <c r="D47" s="99" t="s">
-        <v>215</v>
+        <v>234</v>
       </c>
       <c r="E47" s="104" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F47" s="104" t="s">
         <v>67</v>
       </c>
       <c r="G47" s="105" t="s">
+        <v>230</v>
+      </c>
+      <c r="H47" s="159" t="s">
+        <v>235</v>
+      </c>
+      <c r="I47" s="160"/>
+      <c r="J47" s="160"/>
+      <c r="K47" s="161"/>
+      <c r="L47" s="103" t="s">
+        <v>236</v>
+      </c>
+      <c r="M47" s="103" t="s">
         <v>237</v>
       </c>
-      <c r="H47" s="147" t="s">
-        <v>235</v>
-      </c>
-      <c r="I47" s="148"/>
-      <c r="J47" s="148"/>
-      <c r="K47" s="149"/>
-      <c r="L47" s="103"/>
-      <c r="M47" s="103"/>
       <c r="N47" s="93" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="O47" s="60"/>
       <c r="P47" s="60"/>
     </row>
-    <row r="48" spans="1:16" s="33" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="102">
+    <row r="48" spans="1:16" s="33" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="32">
         <v>44</v>
       </c>
-      <c r="B48" s="102" t="s">
-        <v>219</v>
-      </c>
-      <c r="C48" s="102">
-        <v>51</v>
-      </c>
-      <c r="D48" s="99" t="s">
-        <v>216</v>
-      </c>
-      <c r="E48" s="104" t="s">
-        <v>132</v>
-      </c>
-      <c r="F48" s="104" t="s">
-        <v>67</v>
-      </c>
-      <c r="G48" s="105" t="s">
-        <v>238</v>
-      </c>
-      <c r="H48" s="147" t="s">
-        <v>236</v>
-      </c>
-      <c r="I48" s="148"/>
-      <c r="J48" s="148"/>
-      <c r="K48" s="149"/>
-      <c r="L48" s="103"/>
-      <c r="M48" s="103"/>
-      <c r="N48" s="93" t="s">
-        <v>242</v>
-      </c>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="68"/>
+      <c r="E48" s="59"/>
+      <c r="F48" s="59"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="83"/>
+      <c r="I48" s="84"/>
+      <c r="J48" s="84"/>
+      <c r="K48" s="85"/>
+      <c r="L48" s="81"/>
+      <c r="M48" s="81"/>
+      <c r="N48" s="37"/>
       <c r="O48" s="60"/>
       <c r="P48" s="60"/>
     </row>
-    <row r="49" spans="1:16" s="33" customFormat="1" ht="168.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="102">
+    <row r="49" spans="1:16" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="32">
         <v>45</v>
       </c>
-      <c r="B49" s="102" t="s">
-        <v>219</v>
-      </c>
-      <c r="C49" s="102">
-        <v>51</v>
-      </c>
-      <c r="D49" s="99" t="s">
-        <v>245</v>
-      </c>
-      <c r="E49" s="104" t="s">
-        <v>131</v>
-      </c>
-      <c r="F49" s="104" t="s">
-        <v>67</v>
-      </c>
-      <c r="G49" s="105" t="s">
-        <v>246</v>
-      </c>
-      <c r="H49" s="159" t="s">
-        <v>247</v>
-      </c>
-      <c r="I49" s="160"/>
-      <c r="J49" s="160"/>
-      <c r="K49" s="161"/>
-      <c r="L49" s="103" t="s">
-        <v>248</v>
-      </c>
-      <c r="M49" s="103" t="s">
-        <v>249</v>
-      </c>
-      <c r="N49" s="93" t="s">
-        <v>250</v>
-      </c>
+      <c r="B49" s="32"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="59"/>
+      <c r="F49" s="59"/>
+      <c r="G49" s="37"/>
+      <c r="H49" s="144"/>
+      <c r="I49" s="145"/>
+      <c r="J49" s="145"/>
+      <c r="K49" s="146"/>
+      <c r="L49" s="56"/>
+      <c r="M49" s="56"/>
+      <c r="N49" s="37"/>
       <c r="O49" s="60"/>
       <c r="P49" s="60"/>
     </row>
-    <row r="50" spans="1:16" s="33" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="32">
         <v>46</v>
       </c>
       <c r="B50" s="32"/>
       <c r="C50" s="32"/>
-      <c r="D50" s="68"/>
+      <c r="D50" s="31"/>
       <c r="E50" s="59"/>
       <c r="F50" s="59"/>
       <c r="G50" s="37"/>
-      <c r="H50" s="83"/>
-      <c r="I50" s="84"/>
-      <c r="J50" s="84"/>
-      <c r="K50" s="85"/>
-      <c r="L50" s="81"/>
-      <c r="M50" s="81"/>
+      <c r="H50" s="144"/>
+      <c r="I50" s="145"/>
+      <c r="J50" s="145"/>
+      <c r="K50" s="146"/>
+      <c r="L50" s="56"/>
+      <c r="M50" s="56"/>
       <c r="N50" s="37"/>
       <c r="O50" s="60"/>
       <c r="P50" s="60"/>
@@ -9296,10 +9095,10 @@
       <c r="E51" s="59"/>
       <c r="F51" s="59"/>
       <c r="G51" s="37"/>
-      <c r="H51" s="139"/>
-      <c r="I51" s="140"/>
-      <c r="J51" s="140"/>
-      <c r="K51" s="141"/>
+      <c r="H51" s="144"/>
+      <c r="I51" s="145"/>
+      <c r="J51" s="145"/>
+      <c r="K51" s="146"/>
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
       <c r="N51" s="37"/>
@@ -9316,84 +9115,42 @@
       <c r="E52" s="59"/>
       <c r="F52" s="59"/>
       <c r="G52" s="37"/>
-      <c r="H52" s="139"/>
-      <c r="I52" s="140"/>
-      <c r="J52" s="140"/>
-      <c r="K52" s="141"/>
+      <c r="H52" s="144"/>
+      <c r="I52" s="145"/>
+      <c r="J52" s="145"/>
+      <c r="K52" s="146"/>
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
       <c r="N52" s="37"/>
       <c r="O52" s="60"/>
       <c r="P52" s="60"/>
     </row>
-    <row r="53" spans="1:16" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="32">
-        <v>49</v>
-      </c>
-      <c r="B53" s="32"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="59"/>
-      <c r="F53" s="59"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="139"/>
-      <c r="I53" s="140"/>
-      <c r="J53" s="140"/>
-      <c r="K53" s="141"/>
-      <c r="L53" s="56"/>
-      <c r="M53" s="56"/>
-      <c r="N53" s="37"/>
-      <c r="O53" s="60"/>
-      <c r="P53" s="60"/>
-    </row>
-    <row r="54" spans="1:16" s="33" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="32">
-        <v>50</v>
-      </c>
-      <c r="B54" s="32"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="59"/>
-      <c r="F54" s="59"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="139"/>
-      <c r="I54" s="140"/>
-      <c r="J54" s="140"/>
-      <c r="K54" s="141"/>
-      <c r="L54" s="56"/>
-      <c r="M54" s="56"/>
-      <c r="N54" s="37"/>
-      <c r="O54" s="60"/>
-      <c r="P54" s="60"/>
-    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="18">
+    <mergeCell ref="L5:L17"/>
+    <mergeCell ref="M5:M17"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H22:K33"/>
+    <mergeCell ref="H34:K46"/>
+    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="H52:K52"/>
+    <mergeCell ref="H50:K50"/>
+    <mergeCell ref="H49:K49"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="H4:K4"/>
+    <mergeCell ref="H21:K21"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="H5:K17"/>
     <mergeCell ref="H18:K18"/>
     <mergeCell ref="H19:K19"/>
     <mergeCell ref="H20:K20"/>
-    <mergeCell ref="H54:K54"/>
-    <mergeCell ref="H52:K52"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="H4:K4"/>
-    <mergeCell ref="H21:K21"/>
-    <mergeCell ref="L5:L17"/>
-    <mergeCell ref="M5:M17"/>
-    <mergeCell ref="H53:K53"/>
-    <mergeCell ref="H22:K33"/>
-    <mergeCell ref="H47:K47"/>
-    <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H34:K46"/>
-    <mergeCell ref="H49:K49"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E52">
       <formula1>"Select,Insert,Delete,Update"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F54">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F52">
       <formula1>"SQL Script, ID SQL, ID Store, ID Function, ID Trigger"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9412,7 +9169,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>
@@ -10016,14 +9773,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B1" s="165" t="s">
+      <c r="B1" s="162" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="165"/>
-      <c r="D1" s="165"/>
-      <c r="E1" s="165"/>
-      <c r="F1" s="165"/>
-      <c r="G1" s="165"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
     </row>
     <row r="2" spans="2:7" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2" s="16"/>
@@ -10216,11 +9973,11 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="200.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E27" s="166" t="s">
+      <c r="E27" s="163" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="167"/>
-      <c r="G27" s="168"/>
+      <c r="F27" s="164"/>
+      <c r="G27" s="165"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">

</xml_diff>

<commit_message>
SỬA LẠI CÂU @SQL0001
</commit_message>
<xml_diff>
--- a/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat nguoi dung/AS0053_Cap nhat nhan vien.xlsx
+++ b/2015/201512/10_DOCUMENT/13_DETAIL_DESIGN/Cap nhat nguoi dung/AS0053_Cap nhat nhan vien.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="9990" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="21075" windowHeight="9990" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Update History" sheetId="4" r:id="rId1"/>
@@ -1859,12 +1859,25 @@
     <t xml:space="preserve">EmployeeID, FullName, DepartmentID, EmployeeTypeID, HireDate, EndDate, BirthDay, Address, Tel, Fax, Email, IsUserID, SipID, SipPassword </t>
   </si>
   <si>
-    <t>INSERT INTO AT1103(DivisionID, EmployeeID, FullName,
-      DepartmentID, EmployeeTypeID, HireDate,EndDate,
-      BirthDay,Address, Tel, Fax, Email,IsUserID,Disabled,
-CreateDate,CreateUserID,LastModifyUserID, LastModifyDate,
-      IsCommon) 
-VALUES (@DivisionID, @EmployeeID, @FullName, @DepartmentID, @EmployeeTypeID, @HireDate, @EndDate, @BirthDay, @Address, @Tel, @Fax, @Email, @IsUserID, @SipID, @SipPassword)</t>
+    <t>CustomizeIndex = 51 (Hoàng Trần)
+- Sheet Layout: thêm 2 trường SIP và Mật khẩu
+- Sheet Item Sreen: thêm 5 trường Mật khẩu, Nhập lại mật khẩu, SIP, Mật khẩu và Dùng chung
+- Sheet Data Input: Thêm câu @SQL0001</t>
+  </si>
+  <si>
+    <t>Sửa lại câu SQL Insert into.Thực thi @SQL0001 khi thêm mới một người dùng trong Form AS0053</t>
+  </si>
+  <si>
+    <t>INSERT INTO AT1103( DivisionID,  EmployeeID,
+      FullName, DepartmentID,
+      EmployeeTypeID, HireDate, EndDate,
+      BirthDay,Address, Tel,  Fax, Email,
+      IsUserID,Disabled,CreateDate,  CreateUserID,
+      LastModifyUserID, LastModifyDate,
+      IsCommon, SipID, SipPassword) 
+VALUES (@DivisionID, @EmployeeID, @FullName, @DepartmentID, @EmployeeTypeID, @HireDate, @EndDate, @BirthDay, @Address, @Tel, @Fax, @Email, @IsUserID, @Disabled,@CreateDate,  @CreateUserID,
+      @LastModifyUserID,@LastModifyDate,
+     @IsCommon, @SipID, @SipPassword)</t>
   </si>
   <si>
     <t>@DivisionID
@@ -1874,6 +1887,9 @@
 @Fax 
 @Email
 @IsUserID
+@Disabled @CreateDate @CreateUserID
+@LastModifyUserID@LastModifyDate
+@IsCommon
 @SipID
 @SipPassword</t>
   </si>
@@ -1883,16 +1899,10 @@
 @@Fax
 @@Email 
 @@IsUserID
+@@Disabled GETDATE() @@CreateUserID
+@@LastModifyUserID GETDATE()
+@@IsCommon
 @@SipID @@SipPassword</t>
-  </si>
-  <si>
-    <t>CustomizeIndex = 51 (Hoàng Trần)
-- Sheet Layout: thêm 2 trường SIP và Mật khẩu
-- Sheet Item Sreen: thêm 5 trường Mật khẩu, Nhập lại mật khẩu, SIP, Mật khẩu và Dùng chung
-- Sheet Data Input: Thêm câu @SQL0001</t>
-  </si>
-  <si>
-    <t>Sửa lại câu SQL Insert into.Thực thi @SQL0001 khi thêm mới một người dùng trong Form AS0053</t>
   </si>
 </sst>
 </file>
@@ -2612,6 +2622,24 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2627,6 +2655,42 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2635,60 +2699,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3260,7 +3270,7 @@
         <v>210</v>
       </c>
       <c r="E6" s="111" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="F6" s="112"/>
       <c r="G6" s="112"/>
@@ -3788,23 +3798,15 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="E39:J39"/>
-    <mergeCell ref="E40:J40"/>
-    <mergeCell ref="E41:J41"/>
-    <mergeCell ref="E42:J42"/>
-    <mergeCell ref="E43:J43"/>
-    <mergeCell ref="E38:J38"/>
-    <mergeCell ref="E27:J27"/>
-    <mergeCell ref="E28:J28"/>
-    <mergeCell ref="E29:J29"/>
-    <mergeCell ref="E30:J30"/>
-    <mergeCell ref="E31:J31"/>
-    <mergeCell ref="E37:J37"/>
-    <mergeCell ref="E32:J32"/>
-    <mergeCell ref="E33:J33"/>
-    <mergeCell ref="E34:J34"/>
-    <mergeCell ref="E35:J35"/>
-    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E8:J8"/>
+    <mergeCell ref="E9:J9"/>
+    <mergeCell ref="E10:J10"/>
+    <mergeCell ref="E11:J11"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="E5:J5"/>
+    <mergeCell ref="E6:J6"/>
+    <mergeCell ref="E7:J7"/>
     <mergeCell ref="E12:J12"/>
     <mergeCell ref="E13:J13"/>
     <mergeCell ref="E26:J26"/>
@@ -3820,15 +3822,23 @@
     <mergeCell ref="E23:J23"/>
     <mergeCell ref="E24:J24"/>
     <mergeCell ref="E25:J25"/>
-    <mergeCell ref="E8:J8"/>
-    <mergeCell ref="E9:J9"/>
-    <mergeCell ref="E10:J10"/>
-    <mergeCell ref="E11:J11"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="E5:J5"/>
-    <mergeCell ref="E6:J6"/>
-    <mergeCell ref="E7:J7"/>
+    <mergeCell ref="E38:J38"/>
+    <mergeCell ref="E27:J27"/>
+    <mergeCell ref="E28:J28"/>
+    <mergeCell ref="E29:J29"/>
+    <mergeCell ref="E30:J30"/>
+    <mergeCell ref="E31:J31"/>
+    <mergeCell ref="E37:J37"/>
+    <mergeCell ref="E32:J32"/>
+    <mergeCell ref="E33:J33"/>
+    <mergeCell ref="E34:J34"/>
+    <mergeCell ref="E35:J35"/>
+    <mergeCell ref="E36:J36"/>
+    <mergeCell ref="E39:J39"/>
+    <mergeCell ref="E40:J40"/>
+    <mergeCell ref="E41:J41"/>
+    <mergeCell ref="E42:J42"/>
+    <mergeCell ref="E43:J43"/>
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.6" bottom="0.3" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -7628,8 +7638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P52"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A33" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A44" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H47" sqref="H47:K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7784,13 +7794,13 @@
       <c r="H5" s="118" t="s">
         <v>173</v>
       </c>
-      <c r="I5" s="136"/>
-      <c r="J5" s="136"/>
-      <c r="K5" s="137"/>
-      <c r="L5" s="147" t="s">
+      <c r="I5" s="142"/>
+      <c r="J5" s="142"/>
+      <c r="K5" s="143"/>
+      <c r="L5" s="136" t="s">
         <v>174</v>
       </c>
-      <c r="M5" s="147" t="s">
+      <c r="M5" s="136" t="s">
         <v>188</v>
       </c>
       <c r="N5" s="37"/>
@@ -7813,12 +7823,12 @@
       </c>
       <c r="F6" s="59"/>
       <c r="G6" s="37"/>
-      <c r="H6" s="138"/>
-      <c r="I6" s="139"/>
-      <c r="J6" s="139"/>
-      <c r="K6" s="140"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="145"/>
+      <c r="J6" s="145"/>
+      <c r="K6" s="146"/>
+      <c r="L6" s="137"/>
+      <c r="M6" s="137"/>
       <c r="N6" s="37"/>
       <c r="O6" s="60"/>
       <c r="P6" s="60"/>
@@ -7839,12 +7849,12 @@
       </c>
       <c r="F7" s="59"/>
       <c r="G7" s="37"/>
-      <c r="H7" s="138"/>
-      <c r="I7" s="139"/>
-      <c r="J7" s="139"/>
-      <c r="K7" s="140"/>
-      <c r="L7" s="148"/>
-      <c r="M7" s="148"/>
+      <c r="H7" s="144"/>
+      <c r="I7" s="145"/>
+      <c r="J7" s="145"/>
+      <c r="K7" s="146"/>
+      <c r="L7" s="137"/>
+      <c r="M7" s="137"/>
       <c r="N7" s="37"/>
       <c r="O7" s="60"/>
       <c r="P7" s="60"/>
@@ -7865,12 +7875,12 @@
       </c>
       <c r="F8" s="59"/>
       <c r="G8" s="37"/>
-      <c r="H8" s="138"/>
-      <c r="I8" s="139"/>
-      <c r="J8" s="139"/>
-      <c r="K8" s="140"/>
-      <c r="L8" s="148"/>
-      <c r="M8" s="148"/>
+      <c r="H8" s="144"/>
+      <c r="I8" s="145"/>
+      <c r="J8" s="145"/>
+      <c r="K8" s="146"/>
+      <c r="L8" s="137"/>
+      <c r="M8" s="137"/>
       <c r="N8" s="37"/>
       <c r="O8" s="60"/>
       <c r="P8" s="60"/>
@@ -7891,12 +7901,12 @@
       </c>
       <c r="F9" s="59"/>
       <c r="G9" s="37"/>
-      <c r="H9" s="138"/>
-      <c r="I9" s="139"/>
-      <c r="J9" s="139"/>
-      <c r="K9" s="140"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
+      <c r="H9" s="144"/>
+      <c r="I9" s="145"/>
+      <c r="J9" s="145"/>
+      <c r="K9" s="146"/>
+      <c r="L9" s="137"/>
+      <c r="M9" s="137"/>
       <c r="N9" s="37"/>
       <c r="O9" s="60"/>
       <c r="P9" s="60"/>
@@ -7917,12 +7927,12 @@
       </c>
       <c r="F10" s="59"/>
       <c r="G10" s="37"/>
-      <c r="H10" s="138"/>
-      <c r="I10" s="139"/>
-      <c r="J10" s="139"/>
-      <c r="K10" s="140"/>
-      <c r="L10" s="148"/>
-      <c r="M10" s="148"/>
+      <c r="H10" s="144"/>
+      <c r="I10" s="145"/>
+      <c r="J10" s="145"/>
+      <c r="K10" s="146"/>
+      <c r="L10" s="137"/>
+      <c r="M10" s="137"/>
       <c r="N10" s="37"/>
       <c r="O10" s="60"/>
       <c r="P10" s="60"/>
@@ -7943,12 +7953,12 @@
       </c>
       <c r="F11" s="59"/>
       <c r="G11" s="37"/>
-      <c r="H11" s="138"/>
-      <c r="I11" s="139"/>
-      <c r="J11" s="139"/>
-      <c r="K11" s="140"/>
-      <c r="L11" s="148"/>
-      <c r="M11" s="148"/>
+      <c r="H11" s="144"/>
+      <c r="I11" s="145"/>
+      <c r="J11" s="145"/>
+      <c r="K11" s="146"/>
+      <c r="L11" s="137"/>
+      <c r="M11" s="137"/>
       <c r="N11" s="37"/>
       <c r="O11" s="60"/>
       <c r="P11" s="60"/>
@@ -7969,12 +7979,12 @@
       </c>
       <c r="F12" s="59"/>
       <c r="G12" s="37"/>
-      <c r="H12" s="138"/>
-      <c r="I12" s="139"/>
-      <c r="J12" s="139"/>
-      <c r="K12" s="140"/>
-      <c r="L12" s="148"/>
-      <c r="M12" s="148"/>
+      <c r="H12" s="144"/>
+      <c r="I12" s="145"/>
+      <c r="J12" s="145"/>
+      <c r="K12" s="146"/>
+      <c r="L12" s="137"/>
+      <c r="M12" s="137"/>
       <c r="N12" s="37"/>
       <c r="O12" s="60"/>
       <c r="P12" s="60"/>
@@ -7995,12 +8005,12 @@
       </c>
       <c r="F13" s="59"/>
       <c r="G13" s="37"/>
-      <c r="H13" s="138"/>
-      <c r="I13" s="139"/>
-      <c r="J13" s="139"/>
-      <c r="K13" s="140"/>
-      <c r="L13" s="148"/>
-      <c r="M13" s="148"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="145"/>
+      <c r="J13" s="145"/>
+      <c r="K13" s="146"/>
+      <c r="L13" s="137"/>
+      <c r="M13" s="137"/>
       <c r="N13" s="37"/>
       <c r="O13" s="60"/>
       <c r="P13" s="60"/>
@@ -8021,12 +8031,12 @@
       </c>
       <c r="F14" s="59"/>
       <c r="G14" s="37"/>
-      <c r="H14" s="138"/>
-      <c r="I14" s="139"/>
-      <c r="J14" s="139"/>
-      <c r="K14" s="140"/>
-      <c r="L14" s="148"/>
-      <c r="M14" s="148"/>
+      <c r="H14" s="144"/>
+      <c r="I14" s="145"/>
+      <c r="J14" s="145"/>
+      <c r="K14" s="146"/>
+      <c r="L14" s="137"/>
+      <c r="M14" s="137"/>
       <c r="N14" s="37"/>
       <c r="O14" s="60"/>
       <c r="P14" s="60"/>
@@ -8047,12 +8057,12 @@
       </c>
       <c r="F15" s="59"/>
       <c r="G15" s="37"/>
-      <c r="H15" s="138"/>
-      <c r="I15" s="139"/>
-      <c r="J15" s="139"/>
-      <c r="K15" s="140"/>
-      <c r="L15" s="148"/>
-      <c r="M15" s="148"/>
+      <c r="H15" s="144"/>
+      <c r="I15" s="145"/>
+      <c r="J15" s="145"/>
+      <c r="K15" s="146"/>
+      <c r="L15" s="137"/>
+      <c r="M15" s="137"/>
       <c r="N15" s="37"/>
       <c r="O15" s="60"/>
       <c r="P15" s="60"/>
@@ -8073,12 +8083,12 @@
       </c>
       <c r="F16" s="59"/>
       <c r="G16" s="37"/>
-      <c r="H16" s="138"/>
-      <c r="I16" s="139"/>
-      <c r="J16" s="139"/>
-      <c r="K16" s="140"/>
-      <c r="L16" s="148"/>
-      <c r="M16" s="148"/>
+      <c r="H16" s="144"/>
+      <c r="I16" s="145"/>
+      <c r="J16" s="145"/>
+      <c r="K16" s="146"/>
+      <c r="L16" s="137"/>
+      <c r="M16" s="137"/>
       <c r="N16" s="37"/>
       <c r="O16" s="60"/>
       <c r="P16" s="60"/>
@@ -8099,12 +8109,12 @@
       </c>
       <c r="F17" s="59"/>
       <c r="G17" s="37"/>
-      <c r="H17" s="141"/>
-      <c r="I17" s="142"/>
-      <c r="J17" s="142"/>
-      <c r="K17" s="143"/>
-      <c r="L17" s="149"/>
-      <c r="M17" s="149"/>
+      <c r="H17" s="159"/>
+      <c r="I17" s="160"/>
+      <c r="J17" s="160"/>
+      <c r="K17" s="161"/>
+      <c r="L17" s="138"/>
+      <c r="M17" s="138"/>
       <c r="N17" s="37"/>
       <c r="O17" s="60"/>
       <c r="P17" s="60"/>
@@ -8125,12 +8135,12 @@
       </c>
       <c r="F18" s="59"/>
       <c r="G18" s="37"/>
-      <c r="H18" s="144" t="s">
+      <c r="H18" s="139" t="s">
         <v>206</v>
       </c>
-      <c r="I18" s="145"/>
-      <c r="J18" s="145"/>
-      <c r="K18" s="146"/>
+      <c r="I18" s="140"/>
+      <c r="J18" s="140"/>
+      <c r="K18" s="141"/>
       <c r="L18" s="86"/>
       <c r="M18" s="86"/>
       <c r="N18" s="80" t="s">
@@ -8155,12 +8165,12 @@
       </c>
       <c r="F19" s="59"/>
       <c r="G19" s="37"/>
-      <c r="H19" s="144" t="s">
+      <c r="H19" s="139" t="s">
         <v>207</v>
       </c>
-      <c r="I19" s="145"/>
-      <c r="J19" s="145"/>
-      <c r="K19" s="146"/>
+      <c r="I19" s="140"/>
+      <c r="J19" s="140"/>
+      <c r="K19" s="141"/>
       <c r="L19" s="86"/>
       <c r="M19" s="86"/>
       <c r="N19" s="80" t="s">
@@ -8185,12 +8195,12 @@
       </c>
       <c r="F20" s="59"/>
       <c r="G20" s="37"/>
-      <c r="H20" s="144" t="s">
+      <c r="H20" s="139" t="s">
         <v>208</v>
       </c>
-      <c r="I20" s="145"/>
-      <c r="J20" s="145"/>
-      <c r="K20" s="146"/>
+      <c r="I20" s="140"/>
+      <c r="J20" s="140"/>
+      <c r="K20" s="141"/>
       <c r="L20" s="87" t="s">
         <v>177</v>
       </c>
@@ -8219,12 +8229,12 @@
       </c>
       <c r="F21" s="59"/>
       <c r="G21" s="37"/>
-      <c r="H21" s="144" t="s">
+      <c r="H21" s="139" t="s">
         <v>209</v>
       </c>
-      <c r="I21" s="145"/>
-      <c r="J21" s="145"/>
-      <c r="K21" s="146"/>
+      <c r="I21" s="140"/>
+      <c r="J21" s="140"/>
+      <c r="K21" s="141"/>
       <c r="L21" s="87" t="s">
         <v>178</v>
       </c>
@@ -8256,9 +8266,9 @@
       <c r="H22" s="118" t="s">
         <v>175</v>
       </c>
-      <c r="I22" s="136"/>
-      <c r="J22" s="136"/>
-      <c r="K22" s="137"/>
+      <c r="I22" s="142"/>
+      <c r="J22" s="142"/>
+      <c r="K22" s="143"/>
       <c r="L22" s="81" t="s">
         <v>174</v>
       </c>
@@ -8285,10 +8295,10 @@
       </c>
       <c r="F23" s="59"/>
       <c r="G23" s="37"/>
-      <c r="H23" s="138"/>
-      <c r="I23" s="139"/>
-      <c r="J23" s="139"/>
-      <c r="K23" s="140"/>
+      <c r="H23" s="144"/>
+      <c r="I23" s="145"/>
+      <c r="J23" s="145"/>
+      <c r="K23" s="146"/>
       <c r="L23" s="91" t="s">
         <v>176</v>
       </c>
@@ -8315,10 +8325,10 @@
       </c>
       <c r="F24" s="59"/>
       <c r="G24" s="37"/>
-      <c r="H24" s="138"/>
-      <c r="I24" s="139"/>
-      <c r="J24" s="139"/>
-      <c r="K24" s="140"/>
+      <c r="H24" s="144"/>
+      <c r="I24" s="145"/>
+      <c r="J24" s="145"/>
+      <c r="K24" s="146"/>
       <c r="L24" s="91" t="s">
         <v>177</v>
       </c>
@@ -8345,10 +8355,10 @@
       </c>
       <c r="F25" s="59"/>
       <c r="G25" s="37"/>
-      <c r="H25" s="138"/>
-      <c r="I25" s="139"/>
-      <c r="J25" s="139"/>
-      <c r="K25" s="140"/>
+      <c r="H25" s="144"/>
+      <c r="I25" s="145"/>
+      <c r="J25" s="145"/>
+      <c r="K25" s="146"/>
       <c r="L25" s="91" t="s">
         <v>178</v>
       </c>
@@ -8375,10 +8385,10 @@
       </c>
       <c r="F26" s="59"/>
       <c r="G26" s="37"/>
-      <c r="H26" s="138"/>
-      <c r="I26" s="139"/>
-      <c r="J26" s="139"/>
-      <c r="K26" s="140"/>
+      <c r="H26" s="144"/>
+      <c r="I26" s="145"/>
+      <c r="J26" s="145"/>
+      <c r="K26" s="146"/>
       <c r="L26" s="91" t="s">
         <v>179</v>
       </c>
@@ -8405,10 +8415,10 @@
       </c>
       <c r="F27" s="59"/>
       <c r="G27" s="37"/>
-      <c r="H27" s="138"/>
-      <c r="I27" s="139"/>
-      <c r="J27" s="139"/>
-      <c r="K27" s="140"/>
+      <c r="H27" s="144"/>
+      <c r="I27" s="145"/>
+      <c r="J27" s="145"/>
+      <c r="K27" s="146"/>
       <c r="L27" s="91" t="s">
         <v>180</v>
       </c>
@@ -8435,10 +8445,10 @@
       </c>
       <c r="F28" s="59"/>
       <c r="G28" s="37"/>
-      <c r="H28" s="138"/>
-      <c r="I28" s="139"/>
-      <c r="J28" s="139"/>
-      <c r="K28" s="140"/>
+      <c r="H28" s="144"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
+      <c r="K28" s="146"/>
       <c r="L28" s="91" t="s">
         <v>181</v>
       </c>
@@ -8465,10 +8475,10 @@
       </c>
       <c r="F29" s="59"/>
       <c r="G29" s="37"/>
-      <c r="H29" s="138"/>
-      <c r="I29" s="139"/>
-      <c r="J29" s="139"/>
-      <c r="K29" s="140"/>
+      <c r="H29" s="144"/>
+      <c r="I29" s="145"/>
+      <c r="J29" s="145"/>
+      <c r="K29" s="146"/>
       <c r="L29" s="91" t="s">
         <v>182</v>
       </c>
@@ -8495,10 +8505,10 @@
       </c>
       <c r="F30" s="59"/>
       <c r="G30" s="37"/>
-      <c r="H30" s="138"/>
-      <c r="I30" s="139"/>
-      <c r="J30" s="139"/>
-      <c r="K30" s="140"/>
+      <c r="H30" s="144"/>
+      <c r="I30" s="145"/>
+      <c r="J30" s="145"/>
+      <c r="K30" s="146"/>
       <c r="L30" s="91" t="s">
         <v>183</v>
       </c>
@@ -8525,10 +8535,10 @@
       </c>
       <c r="F31" s="59"/>
       <c r="G31" s="37"/>
-      <c r="H31" s="138"/>
-      <c r="I31" s="139"/>
-      <c r="J31" s="139"/>
-      <c r="K31" s="140"/>
+      <c r="H31" s="144"/>
+      <c r="I31" s="145"/>
+      <c r="J31" s="145"/>
+      <c r="K31" s="146"/>
       <c r="L31" s="91" t="s">
         <v>184</v>
       </c>
@@ -8555,10 +8565,10 @@
       </c>
       <c r="F32" s="59"/>
       <c r="G32" s="37"/>
-      <c r="H32" s="138"/>
-      <c r="I32" s="139"/>
-      <c r="J32" s="139"/>
-      <c r="K32" s="140"/>
+      <c r="H32" s="144"/>
+      <c r="I32" s="145"/>
+      <c r="J32" s="145"/>
+      <c r="K32" s="146"/>
       <c r="L32" s="91" t="s">
         <v>185</v>
       </c>
@@ -8585,10 +8595,10 @@
       </c>
       <c r="F33" s="59"/>
       <c r="G33" s="37"/>
-      <c r="H33" s="138"/>
-      <c r="I33" s="139"/>
-      <c r="J33" s="139"/>
-      <c r="K33" s="140"/>
+      <c r="H33" s="144"/>
+      <c r="I33" s="145"/>
+      <c r="J33" s="145"/>
+      <c r="K33" s="146"/>
       <c r="L33" s="91" t="s">
         <v>186</v>
       </c>
@@ -8615,12 +8625,12 @@
       </c>
       <c r="F34" s="59"/>
       <c r="G34" s="37"/>
-      <c r="H34" s="150" t="s">
+      <c r="H34" s="147" t="s">
         <v>199</v>
       </c>
-      <c r="I34" s="151"/>
-      <c r="J34" s="151"/>
-      <c r="K34" s="152"/>
+      <c r="I34" s="148"/>
+      <c r="J34" s="148"/>
+      <c r="K34" s="149"/>
       <c r="L34" s="91" t="s">
         <v>176</v>
       </c>
@@ -8647,10 +8657,10 @@
       </c>
       <c r="F35" s="59"/>
       <c r="G35" s="37"/>
-      <c r="H35" s="153"/>
-      <c r="I35" s="154"/>
-      <c r="J35" s="154"/>
-      <c r="K35" s="155"/>
+      <c r="H35" s="150"/>
+      <c r="I35" s="151"/>
+      <c r="J35" s="151"/>
+      <c r="K35" s="152"/>
       <c r="L35" s="91" t="s">
         <v>177</v>
       </c>
@@ -8677,10 +8687,10 @@
       </c>
       <c r="F36" s="59"/>
       <c r="G36" s="37"/>
-      <c r="H36" s="153"/>
-      <c r="I36" s="154"/>
-      <c r="J36" s="154"/>
-      <c r="K36" s="155"/>
+      <c r="H36" s="150"/>
+      <c r="I36" s="151"/>
+      <c r="J36" s="151"/>
+      <c r="K36" s="152"/>
       <c r="L36" s="91" t="s">
         <v>178</v>
       </c>
@@ -8707,10 +8717,10 @@
       </c>
       <c r="F37" s="59"/>
       <c r="G37" s="37"/>
-      <c r="H37" s="153"/>
-      <c r="I37" s="154"/>
-      <c r="J37" s="154"/>
-      <c r="K37" s="155"/>
+      <c r="H37" s="150"/>
+      <c r="I37" s="151"/>
+      <c r="J37" s="151"/>
+      <c r="K37" s="152"/>
       <c r="L37" s="91" t="s">
         <v>179</v>
       </c>
@@ -8737,10 +8747,10 @@
       </c>
       <c r="F38" s="59"/>
       <c r="G38" s="37"/>
-      <c r="H38" s="153"/>
-      <c r="I38" s="154"/>
-      <c r="J38" s="154"/>
-      <c r="K38" s="155"/>
+      <c r="H38" s="150"/>
+      <c r="I38" s="151"/>
+      <c r="J38" s="151"/>
+      <c r="K38" s="152"/>
       <c r="L38" s="91" t="s">
         <v>180</v>
       </c>
@@ -8767,10 +8777,10 @@
       </c>
       <c r="F39" s="59"/>
       <c r="G39" s="37"/>
-      <c r="H39" s="153"/>
-      <c r="I39" s="154"/>
-      <c r="J39" s="154"/>
-      <c r="K39" s="155"/>
+      <c r="H39" s="150"/>
+      <c r="I39" s="151"/>
+      <c r="J39" s="151"/>
+      <c r="K39" s="152"/>
       <c r="L39" s="91" t="s">
         <v>181</v>
       </c>
@@ -8797,10 +8807,10 @@
       </c>
       <c r="F40" s="59"/>
       <c r="G40" s="37"/>
-      <c r="H40" s="153"/>
-      <c r="I40" s="154"/>
-      <c r="J40" s="154"/>
-      <c r="K40" s="155"/>
+      <c r="H40" s="150"/>
+      <c r="I40" s="151"/>
+      <c r="J40" s="151"/>
+      <c r="K40" s="152"/>
       <c r="L40" s="91" t="s">
         <v>182</v>
       </c>
@@ -8827,10 +8837,10 @@
       </c>
       <c r="F41" s="59"/>
       <c r="G41" s="37"/>
-      <c r="H41" s="153"/>
-      <c r="I41" s="154"/>
-      <c r="J41" s="154"/>
-      <c r="K41" s="155"/>
+      <c r="H41" s="150"/>
+      <c r="I41" s="151"/>
+      <c r="J41" s="151"/>
+      <c r="K41" s="152"/>
       <c r="L41" s="91" t="s">
         <v>183</v>
       </c>
@@ -8857,10 +8867,10 @@
       </c>
       <c r="F42" s="59"/>
       <c r="G42" s="37"/>
-      <c r="H42" s="153"/>
-      <c r="I42" s="154"/>
-      <c r="J42" s="154"/>
-      <c r="K42" s="155"/>
+      <c r="H42" s="150"/>
+      <c r="I42" s="151"/>
+      <c r="J42" s="151"/>
+      <c r="K42" s="152"/>
       <c r="L42" s="91" t="s">
         <v>184</v>
       </c>
@@ -8887,10 +8897,10 @@
       </c>
       <c r="F43" s="59"/>
       <c r="G43" s="37"/>
-      <c r="H43" s="153"/>
-      <c r="I43" s="154"/>
-      <c r="J43" s="154"/>
-      <c r="K43" s="155"/>
+      <c r="H43" s="150"/>
+      <c r="I43" s="151"/>
+      <c r="J43" s="151"/>
+      <c r="K43" s="152"/>
       <c r="L43" s="91" t="s">
         <v>185</v>
       </c>
@@ -8917,10 +8927,10 @@
       </c>
       <c r="F44" s="59"/>
       <c r="G44" s="37"/>
-      <c r="H44" s="153"/>
-      <c r="I44" s="154"/>
-      <c r="J44" s="154"/>
-      <c r="K44" s="155"/>
+      <c r="H44" s="150"/>
+      <c r="I44" s="151"/>
+      <c r="J44" s="151"/>
+      <c r="K44" s="152"/>
       <c r="L44" s="91" t="s">
         <v>186</v>
       </c>
@@ -8947,10 +8957,10 @@
       </c>
       <c r="F45" s="59"/>
       <c r="G45" s="37"/>
-      <c r="H45" s="153"/>
-      <c r="I45" s="154"/>
-      <c r="J45" s="154"/>
-      <c r="K45" s="155"/>
+      <c r="H45" s="150"/>
+      <c r="I45" s="151"/>
+      <c r="J45" s="151"/>
+      <c r="K45" s="152"/>
       <c r="L45" s="91" t="s">
         <v>133</v>
       </c>
@@ -8971,10 +8981,10 @@
       <c r="E46" s="59"/>
       <c r="F46" s="59"/>
       <c r="G46" s="37"/>
-      <c r="H46" s="156"/>
-      <c r="I46" s="157"/>
-      <c r="J46" s="157"/>
-      <c r="K46" s="158"/>
+      <c r="H46" s="153"/>
+      <c r="I46" s="154"/>
+      <c r="J46" s="154"/>
+      <c r="K46" s="155"/>
       <c r="L46" s="81" t="s">
         <v>174</v>
       </c>
@@ -8985,7 +8995,7 @@
       <c r="O46" s="60"/>
       <c r="P46" s="60"/>
     </row>
-    <row r="47" spans="1:16" s="33" customFormat="1" ht="168.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="33" customFormat="1" ht="236.25" x14ac:dyDescent="0.25">
       <c r="A47" s="32">
         <v>43</v>
       </c>
@@ -9007,20 +9017,20 @@
       <c r="G47" s="105" t="s">
         <v>230</v>
       </c>
-      <c r="H47" s="159" t="s">
-        <v>235</v>
-      </c>
-      <c r="I47" s="160"/>
-      <c r="J47" s="160"/>
-      <c r="K47" s="161"/>
+      <c r="H47" s="156" t="s">
+        <v>237</v>
+      </c>
+      <c r="I47" s="157"/>
+      <c r="J47" s="157"/>
+      <c r="K47" s="158"/>
       <c r="L47" s="103" t="s">
+        <v>238</v>
+      </c>
+      <c r="M47" s="103" t="s">
+        <v>239</v>
+      </c>
+      <c r="N47" s="93" t="s">
         <v>236</v>
-      </c>
-      <c r="M47" s="103" t="s">
-        <v>237</v>
-      </c>
-      <c r="N47" s="93" t="s">
-        <v>239</v>
       </c>
       <c r="O47" s="60"/>
       <c r="P47" s="60"/>
@@ -9055,10 +9065,10 @@
       <c r="E49" s="59"/>
       <c r="F49" s="59"/>
       <c r="G49" s="37"/>
-      <c r="H49" s="144"/>
-      <c r="I49" s="145"/>
-      <c r="J49" s="145"/>
-      <c r="K49" s="146"/>
+      <c r="H49" s="139"/>
+      <c r="I49" s="140"/>
+      <c r="J49" s="140"/>
+      <c r="K49" s="141"/>
       <c r="L49" s="56"/>
       <c r="M49" s="56"/>
       <c r="N49" s="37"/>
@@ -9075,10 +9085,10 @@
       <c r="E50" s="59"/>
       <c r="F50" s="59"/>
       <c r="G50" s="37"/>
-      <c r="H50" s="144"/>
-      <c r="I50" s="145"/>
-      <c r="J50" s="145"/>
-      <c r="K50" s="146"/>
+      <c r="H50" s="139"/>
+      <c r="I50" s="140"/>
+      <c r="J50" s="140"/>
+      <c r="K50" s="141"/>
       <c r="L50" s="56"/>
       <c r="M50" s="56"/>
       <c r="N50" s="37"/>
@@ -9095,10 +9105,10 @@
       <c r="E51" s="59"/>
       <c r="F51" s="59"/>
       <c r="G51" s="37"/>
-      <c r="H51" s="144"/>
-      <c r="I51" s="145"/>
-      <c r="J51" s="145"/>
-      <c r="K51" s="146"/>
+      <c r="H51" s="139"/>
+      <c r="I51" s="140"/>
+      <c r="J51" s="140"/>
+      <c r="K51" s="141"/>
       <c r="L51" s="56"/>
       <c r="M51" s="56"/>
       <c r="N51" s="37"/>
@@ -9115,10 +9125,10 @@
       <c r="E52" s="59"/>
       <c r="F52" s="59"/>
       <c r="G52" s="37"/>
-      <c r="H52" s="144"/>
-      <c r="I52" s="145"/>
-      <c r="J52" s="145"/>
-      <c r="K52" s="146"/>
+      <c r="H52" s="139"/>
+      <c r="I52" s="140"/>
+      <c r="J52" s="140"/>
+      <c r="K52" s="141"/>
       <c r="L52" s="56"/>
       <c r="M52" s="56"/>
       <c r="N52" s="37"/>
@@ -9127,12 +9137,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="L5:L17"/>
-    <mergeCell ref="M5:M17"/>
-    <mergeCell ref="H51:K51"/>
-    <mergeCell ref="H22:K33"/>
-    <mergeCell ref="H34:K46"/>
-    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="A1:E2"/>
+    <mergeCell ref="H5:K17"/>
+    <mergeCell ref="H18:K18"/>
+    <mergeCell ref="H19:K19"/>
+    <mergeCell ref="H20:K20"/>
     <mergeCell ref="H52:K52"/>
     <mergeCell ref="H50:K50"/>
     <mergeCell ref="H49:K49"/>
@@ -9140,11 +9149,12 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="H4:K4"/>
     <mergeCell ref="H21:K21"/>
-    <mergeCell ref="A1:E2"/>
-    <mergeCell ref="H5:K17"/>
-    <mergeCell ref="H18:K18"/>
-    <mergeCell ref="H19:K19"/>
-    <mergeCell ref="H20:K20"/>
+    <mergeCell ref="L5:L17"/>
+    <mergeCell ref="M5:M17"/>
+    <mergeCell ref="H51:K51"/>
+    <mergeCell ref="H22:K33"/>
+    <mergeCell ref="H34:K46"/>
+    <mergeCell ref="H47:K47"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E52">
@@ -9169,7 +9179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J45"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>